<commit_message>
17.06 - LastUpdate- Prezentare
</commit_message>
<xml_diff>
--- a/Documentatie/RezultateExperimentale/W4W5_TerasaCameraSeara_CameraAerisita_Ne_0102_06.xlsx
+++ b/Documentatie/RezultateExperimentale/W4W5_TerasaCameraSeara_CameraAerisita_Ne_0102_06.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="630" windowWidth="19575" windowHeight="7380" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="720" yWindow="630" windowWidth="19575" windowHeight="7380" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="W4W5_TerasaCameraSeara_CameraAe" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2307" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2314" uniqueCount="32">
   <si>
     <t>Device</t>
   </si>
@@ -104,6 +104,19 @@
   </si>
   <si>
     <t>2/6/2020  2:12:52 AM - W5 Cam. Deschisa</t>
+  </si>
+  <si>
+    <t>2/6/2020  12:48:22 PM - Cam.Deschisa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W4(σ)
+</t>
+  </si>
+  <si>
+    <t>W5(σ)</t>
+  </si>
+  <si>
+    <t>σ</t>
   </si>
 </sst>
 </file>
@@ -594,7 +607,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -605,6 +618,9 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="22" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1811,24 +1827,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="108870656"/>
-        <c:axId val="109830912"/>
+        <c:axId val="129895424"/>
+        <c:axId val="129897216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="108870656"/>
+        <c:axId val="129895424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109830912"/>
+        <c:crossAx val="129897216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="109830912"/>
+        <c:axId val="129897216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1836,7 +1852,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108870656"/>
+        <c:crossAx val="129895424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1848,7 +1864,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1858,9 +1874,7 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:title>
-      <c:layout/>
-    </c:title>
+    <c:title/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -2447,24 +2461,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="166388096"/>
-        <c:axId val="166389632"/>
+        <c:axId val="132129152"/>
+        <c:axId val="132130688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="166388096"/>
+        <c:axId val="132129152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166389632"/>
+        <c:crossAx val="132130688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="166389632"/>
+        <c:axId val="132130688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="100"/>
@@ -2473,20 +2487,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166388096"/>
+        <c:crossAx val="132129152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2496,9 +2509,7 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:title>
-      <c:layout/>
-    </c:title>
+    <c:title/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -3085,24 +3096,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="166922496"/>
-        <c:axId val="181288960"/>
+        <c:axId val="132167936"/>
+        <c:axId val="132169728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="166922496"/>
+        <c:axId val="132167936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181288960"/>
+        <c:crossAx val="132169728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="181288960"/>
+        <c:axId val="132169728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3110,20 +3121,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166922496"/>
+        <c:crossAx val="132167936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3139,9 +3149,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.4762070304125975E-2"/>
+          <c:x val="4.4762070304125996E-2"/>
           <c:y val="5.1400554097404488E-2"/>
-          <c:w val="0.84629747440510406"/>
+          <c:w val="0.84629747440510428"/>
           <c:h val="0.56604950422863864"/>
         </c:manualLayout>
       </c:layout>
@@ -4310,24 +4320,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="181303168"/>
-        <c:axId val="181304704"/>
+        <c:axId val="132073344"/>
+        <c:axId val="132074880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="181303168"/>
+        <c:axId val="132073344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181304704"/>
+        <c:crossAx val="132074880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="181304704"/>
+        <c:axId val="132074880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="10"/>
@@ -4336,20 +4346,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181303168"/>
+        <c:crossAx val="132073344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4946,24 +4955,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="181525888"/>
-        <c:axId val="181675136"/>
+        <c:axId val="132087168"/>
+        <c:axId val="132117632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="181525888"/>
+        <c:axId val="132087168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181675136"/>
+        <c:crossAx val="132117632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="181675136"/>
+        <c:axId val="132117632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4971,7 +4980,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181525888"/>
+        <c:crossAx val="132087168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4983,7 +4992,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5580,24 +5589,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="181704192"/>
-        <c:axId val="181705728"/>
+        <c:axId val="132208128"/>
+        <c:axId val="132209664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="181704192"/>
+        <c:axId val="132208128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181705728"/>
+        <c:crossAx val="132209664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="181705728"/>
+        <c:axId val="132209664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="68"/>
@@ -5607,7 +5616,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181704192"/>
+        <c:crossAx val="132208128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5619,7 +5628,184 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>FormuleW4!$B$50</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>W4(σ)
+</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>FormuleW4!$A$51:$A$54</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>CO</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>NO2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SO2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>O3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>FormuleW4!$B$51:$B$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10095</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>356</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1618</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>630</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>FormuleW4!$C$50</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>W5(σ)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>FormuleW4!$A$51:$A$54</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>CO</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>NO2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SO2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>O3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>FormuleW4!$C$51:$C$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>908</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>635</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1230</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>670</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="113469312"/>
+        <c:axId val="113476736"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="113469312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="113476736"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="113476736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2000"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="113469312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1200" baseline="0"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6780,24 +6966,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="109879680"/>
-        <c:axId val="109881216"/>
+        <c:axId val="129942272"/>
+        <c:axId val="129943808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="109879680"/>
+        <c:axId val="129942272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109881216"/>
+        <c:crossAx val="129943808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="109881216"/>
+        <c:axId val="129943808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6805,7 +6991,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109879680"/>
+        <c:crossAx val="129942272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6817,7 +7003,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7978,24 +8164,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="110163456"/>
-        <c:axId val="110164992"/>
+        <c:axId val="130697088"/>
+        <c:axId val="130698624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="110163456"/>
+        <c:axId val="130697088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="t"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110164992"/>
+        <c:crossAx val="130698624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110164992"/>
+        <c:axId val="130698624"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -8003,7 +8189,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110163456"/>
+        <c:crossAx val="130697088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8015,7 +8201,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8175,7 +8361,7 @@
                   <c:v>2/6/2020 11:08</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2/6/2020  12:48:22 PM - W4 Cam.Deschisa</c:v>
+                  <c:v>2/6/2020  12:48:22 PM - Cam.Deschisa</c:v>
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>2/6/2020 12:49</c:v>
@@ -8632,24 +8818,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="117321728"/>
-        <c:axId val="117323264"/>
+        <c:axId val="130769280"/>
+        <c:axId val="130770816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="117321728"/>
+        <c:axId val="130769280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117323264"/>
+        <c:crossAx val="130770816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="117323264"/>
+        <c:axId val="130770816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8657,7 +8843,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117321728"/>
+        <c:crossAx val="130769280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8670,7 +8856,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8830,7 +9016,7 @@
                   <c:v>2/6/2020 11:08</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2/6/2020  12:48:22 PM - W4 Cam.Deschisa</c:v>
+                  <c:v>2/6/2020  12:48:22 PM - Cam.Deschisa</c:v>
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>2/6/2020 12:49</c:v>
@@ -9287,24 +9473,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="117553024"/>
-        <c:axId val="117554560"/>
+        <c:axId val="130795776"/>
+        <c:axId val="130797568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="117553024"/>
+        <c:axId val="130795776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117554560"/>
+        <c:crossAx val="130797568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="117554560"/>
+        <c:axId val="130797568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="100"/>
@@ -9313,7 +9499,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117553024"/>
+        <c:crossAx val="130795776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9326,7 +9512,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -9486,7 +9672,7 @@
                   <c:v>2/6/2020 11:08</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2/6/2020  12:48:22 PM - W4 Cam.Deschisa</c:v>
+                  <c:v>2/6/2020  12:48:22 PM - Cam.Deschisa</c:v>
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>2/6/2020 12:49</c:v>
@@ -9943,24 +10129,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="155869184"/>
-        <c:axId val="155870720"/>
+        <c:axId val="130830720"/>
+        <c:axId val="130832256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="155869184"/>
+        <c:axId val="130830720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="155870720"/>
+        <c:crossAx val="130832256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="155870720"/>
+        <c:axId val="130832256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9968,7 +10154,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="155869184"/>
+        <c:crossAx val="130830720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9981,7 +10167,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -10141,7 +10327,7 @@
                   <c:v>2/6/2020 11:08</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2/6/2020  12:48:22 PM - W4 Cam.Deschisa</c:v>
+                  <c:v>2/6/2020  12:48:22 PM - Cam.Deschisa</c:v>
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>2/6/2020 12:49</c:v>
@@ -10598,24 +10784,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="161351552"/>
-        <c:axId val="161353088"/>
+        <c:axId val="130844928"/>
+        <c:axId val="130859008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="161351552"/>
+        <c:axId val="130844928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="161353088"/>
+        <c:crossAx val="130859008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="161353088"/>
+        <c:axId val="130859008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10623,7 +10809,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="161351552"/>
+        <c:crossAx val="130844928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10636,7 +10822,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -10646,9 +10832,7 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:title>
-      <c:layout/>
-    </c:title>
+    <c:title/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -11235,24 +11419,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="166306176"/>
-        <c:axId val="166307712"/>
+        <c:axId val="131002752"/>
+        <c:axId val="131004288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="166306176"/>
+        <c:axId val="131002752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166307712"/>
+        <c:crossAx val="131004288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="166307712"/>
+        <c:axId val="131004288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11260,20 +11444,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166306176"/>
+        <c:crossAx val="131002752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -11283,9 +11466,7 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:title>
-      <c:layout/>
-    </c:title>
+    <c:title/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -11872,24 +12053,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="166340864"/>
-        <c:axId val="166359040"/>
+        <c:axId val="130918656"/>
+        <c:axId val="130920448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="166340864"/>
+        <c:axId val="130918656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166359040"/>
+        <c:crossAx val="130920448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="166359040"/>
+        <c:axId val="130920448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11897,20 +12078,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166340864"/>
+        <c:crossAx val="130918656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -12351,6 +12531,41 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>303557</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>87382</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>611670</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>163582</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -55325,8 +55540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView topLeftCell="J66" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N83" sqref="N83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -57266,7 +57481,7 @@
         <v>17</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C42" s="3">
         <v>500</v>
@@ -64391,10 +64606,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O55"/>
+  <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -64884,48 +65099,64 @@
         <v>2822241</v>
       </c>
     </row>
-    <row r="48" spans="3:7">
-      <c r="G48">
-        <v>2820887</v>
-      </c>
-    </row>
-    <row r="49" spans="7:7">
-      <c r="G49">
-        <v>2819843</v>
-      </c>
-    </row>
-    <row r="50" spans="7:7">
-      <c r="G50">
-        <v>2818889</v>
-      </c>
-    </row>
-    <row r="51" spans="7:7">
-      <c r="G51">
-        <v>2818147</v>
-      </c>
-    </row>
-    <row r="52" spans="7:7">
-      <c r="G52">
-        <v>2817489</v>
-      </c>
-    </row>
-    <row r="53" spans="7:7">
-      <c r="G53">
-        <v>2816858</v>
-      </c>
-    </row>
-    <row r="54" spans="7:7">
-      <c r="G54">
-        <v>2816268</v>
-      </c>
-    </row>
-    <row r="55" spans="7:7">
-      <c r="G55">
-        <v>2816268</v>
+    <row r="50" spans="1:5" ht="30">
+      <c r="B50" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C50" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>2</v>
+      </c>
+      <c r="B51">
+        <v>10095</v>
+      </c>
+      <c r="C51">
+        <v>908</v>
+      </c>
+      <c r="E51" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>3</v>
+      </c>
+      <c r="B52">
+        <v>356</v>
+      </c>
+      <c r="C52">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53">
+        <v>1618</v>
+      </c>
+      <c r="C53">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54">
+        <v>630</v>
+      </c>
+      <c r="C54">
+        <v>670</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>